<commit_message>
Ajout du fichier excel
</commit_message>
<xml_diff>
--- a/Rapport d'activite╠üs.xlsx
+++ b/Rapport d'activite╠üs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/Documents_locaux/enseignement/A22/Mono2/working/tps/tp2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automne-2022-Limoilou\Automne2022\AppMonoposte\Travaux\TP2_final\a22-mathAssis-pm-rd-ih\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E139A9-FF13-8E45-9478-32B032E769D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD184BE0-F87D-4E80-8B26-A93E501B6778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="28520" windowHeight="18500" xr2:uid="{B02FC5E5-3D9B-7A4B-82B9-DDD6D5EB7D75}"/>
+    <workbookView xWindow="5295" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{B02FC5E5-3D9B-7A4B-82B9-DDD6D5EB7D75}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>Développeur</t>
   </si>
@@ -51,18 +51,6 @@
   </si>
   <si>
     <t>développeur 3:</t>
-  </si>
-  <si>
-    <t>nom1</t>
-  </si>
-  <si>
-    <t>nom2</t>
-  </si>
-  <si>
-    <t>nom3</t>
-  </si>
-  <si>
-    <t>nom4</t>
   </si>
   <si>
     <t xml:space="preserve">Description </t>
@@ -264,6 +252,120 @@
       </rPr>
       <t xml:space="preserve"> :Au moins un plugin</t>
     </r>
+  </si>
+  <si>
+    <t>Patrick Messier</t>
+  </si>
+  <si>
+    <t>Rose Duval</t>
+  </si>
+  <si>
+    <t>Ibrahim Hamitouche</t>
+  </si>
+  <si>
+    <t>toto</t>
+  </si>
+  <si>
+    <t>1 Recursive qui calcul le nombre de sous dossiers dans un dossier recu en param</t>
+  </si>
+  <si>
+    <t>controller/statistique constroller</t>
+  </si>
+  <si>
+    <t>Progress bar dans fonction personnel</t>
+  </si>
+  <si>
+    <t>controller/AvisController</t>
+  </si>
+  <si>
+    <t>controller/EditeurEquationController</t>
+  </si>
+  <si>
+    <t>Controller/AvisController</t>
+  </si>
+  <si>
+    <t>Controller/MainController</t>
+  </si>
+  <si>
+    <t>Stream qui remplis une listView utilisation de collect</t>
+  </si>
+  <si>
+    <t>Stream qui remplis une listView utilisation de Map</t>
+  </si>
+  <si>
+    <t>lecture fichier remplir tree view</t>
+  </si>
+  <si>
+    <t>Cellule personalisé</t>
+  </si>
+  <si>
+    <t>Possibilité de changer une data avec le line chart</t>
+  </si>
+  <si>
+    <t>Vue/Traceur Graphique</t>
+  </si>
+  <si>
+    <t>Controller/CustomTreeCell</t>
+  </si>
+  <si>
+    <t>modele/Recursive</t>
+  </si>
+  <si>
+    <t>Calcul data</t>
+  </si>
+  <si>
+    <t>Modele/Serie</t>
+  </si>
+  <si>
+    <t>calcul nombre équation et séries meme catégorie pureRec</t>
+  </si>
+  <si>
+    <t>Service avec une barre d'animation lors du troquage de Data</t>
+  </si>
+  <si>
+    <t>Vue/TronqueurBarService</t>
+  </si>
+  <si>
+    <t>Service qui ajoute un par un les nouvelles Data dans la nouvelle ListeView</t>
+  </si>
+  <si>
+    <t>Vue/TronqueurService</t>
+  </si>
+  <si>
+    <t>Controller/Service</t>
+  </si>
+  <si>
+    <t>Nombre de temps dans app Service</t>
+  </si>
+  <si>
+    <t>Animation fenetres lors de l'ouverture</t>
+  </si>
+  <si>
+    <t>Stream pour obtenir le nom des séries sélectionné</t>
+  </si>
+  <si>
+    <t>Controller/TronqueurController</t>
+  </si>
+  <si>
+    <t>Stream qui transforme les données recu de la vie en nouvelle série</t>
+  </si>
+  <si>
+    <t>Modele/tronqueur</t>
+  </si>
+  <si>
+    <t>Controller/TreeViewBinaireController</t>
+  </si>
+  <si>
+    <t>Stream qui va chercher les élements en BD vers la liste view</t>
+  </si>
+  <si>
+    <t>Stream qui va chercher les catégories en BD et les transforme en TreeItem</t>
+  </si>
+  <si>
+    <t>Travail en équipe tous les soirs de la semaine</t>
+  </si>
+  <si>
+    <t>Travail en équipe tous les soirs de la semaine(un peu moins que les autres)</t>
   </si>
 </sst>
 </file>
@@ -372,13 +474,7 @@
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -388,14 +484,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,9 +516,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -454,7 +556,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -560,7 +662,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -712,571 +814,622 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A35C1B-8463-5A47-9719-955374213ED5}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="84" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.125" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>B56</f>
-        <v>nom1</v>
-      </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="8">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Patrick Messier</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>B57</f>
-        <v>nom2</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="8">
-        <v>2</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Rose Duval</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>B58</f>
-        <v>nom3</v>
-      </c>
-      <c r="B8" s="8">
+        <v>Ibrahim Hamitouche</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>B59</f>
+        <v>toto</v>
+      </c>
+      <c r="B10" s="6">
         <v>1</v>
       </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="8">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
         <v>2</v>
       </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="str">
-        <f t="shared" ref="A10" si="0">B59</f>
-        <v>nom4</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="8">
-        <v>2</v>
-      </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>9</v>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>B56</f>
-        <v>nom1</v>
-      </c>
-      <c r="B14" s="8">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Patrick Messier</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>B57</f>
-        <v>nom2</v>
-      </c>
-      <c r="B15" s="8">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Rose Duval</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>B58</f>
-        <v>nom3</v>
-      </c>
-      <c r="B16" s="8">
+        <v>Ibrahim Hamitouche</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>B59</f>
+        <v>toto</v>
+      </c>
+      <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="str">
-        <f t="shared" ref="A17" si="1">B59</f>
-        <v>nom4</v>
-      </c>
-      <c r="B17" s="8">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>9</v>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>B56</f>
-        <v>nom1</v>
-      </c>
-      <c r="B20" s="8">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="8">
+        <v>Patrick Messier</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
         <v>2</v>
       </c>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>B57</f>
-        <v>nom2</v>
-      </c>
-      <c r="B22" s="8">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="8">
+        <v>Rose Duval</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
         <v>2</v>
       </c>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>B58</f>
-        <v>nom3</v>
-      </c>
-      <c r="B24" s="8">
+        <v>Ibrahim Hamitouche</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>2</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>B59</f>
+        <v>toto</v>
+      </c>
+      <c r="B26" s="6">
         <v>1</v>
       </c>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="8">
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
         <v>2</v>
       </c>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="str">
-        <f t="shared" ref="A26" si="2">B59</f>
-        <v>nom4</v>
-      </c>
-      <c r="B26" s="8">
-        <v>1</v>
-      </c>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="8">
-        <v>2</v>
-      </c>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="3" t="s">
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>9</v>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>B56</f>
-        <v>nom1</v>
-      </c>
-      <c r="B30" s="8">
-        <v>1</v>
-      </c>
-      <c r="D30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="8">
-        <v>2</v>
-      </c>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>Patrick Messier</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>B57</f>
-        <v>nom2</v>
-      </c>
-      <c r="B32" s="8">
-        <v>1</v>
-      </c>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="8">
-        <v>2</v>
-      </c>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Rose Duval</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>B58</f>
-        <v>nom3</v>
-      </c>
-      <c r="B34" s="8">
+        <v>Ibrahim Hamitouche</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>B59</f>
+        <v>toto</v>
+      </c>
+      <c r="B36" s="6">
         <v>1</v>
       </c>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="8">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
         <v>2</v>
       </c>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="str">
-        <f t="shared" ref="A36" si="3">B59</f>
-        <v>nom4</v>
-      </c>
-      <c r="B36" s="8">
-        <v>1</v>
-      </c>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="8">
-        <v>2</v>
-      </c>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B38" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>9</v>
+      <c r="B39" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>B56</f>
-        <v>nom1</v>
-      </c>
-      <c r="B40" s="8">
+        <v>Patrick Messier</v>
+      </c>
+      <c r="B40" s="6">
         <v>1</v>
       </c>
-      <c r="D40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>B57</f>
-        <v>nom2</v>
-      </c>
-      <c r="B41" s="8">
+        <v>Rose Duval</v>
+      </c>
+      <c r="B41" s="6">
         <v>1</v>
       </c>
-      <c r="D41" s="6"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>B58</f>
-        <v>nom3</v>
-      </c>
-      <c r="B42" s="8">
+        <v>Ibrahim Hamitouche</v>
+      </c>
+      <c r="B42" s="6">
         <v>1</v>
       </c>
-      <c r="D42" s="6"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" ref="A43" si="4">B59</f>
-        <v>nom4</v>
-      </c>
-      <c r="B43" s="8">
+        <f>B59</f>
+        <v>toto</v>
+      </c>
+      <c r="B43" s="6">
         <v>1</v>
       </c>
-      <c r="D43" s="6"/>
-    </row>
-    <row r="44" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B44" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>9</v>
+      <c r="B45" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>B56</f>
-        <v>nom1</v>
-      </c>
-      <c r="B46" s="8">
+        <v>Patrick Messier</v>
+      </c>
+      <c r="B46" s="6">
         <v>1</v>
       </c>
-      <c r="D46" s="6"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" ref="A47:A49" si="5">B57</f>
-        <v>nom2</v>
-      </c>
-      <c r="B47" s="8">
+        <f t="shared" ref="A47" si="0">B57</f>
+        <v>Rose Duval</v>
+      </c>
+      <c r="B47" s="6">
         <v>1</v>
       </c>
-      <c r="D47" s="6"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f t="shared" si="5"/>
-        <v>nom3</v>
-      </c>
-      <c r="B48" s="8">
+        <f>B58</f>
+        <v>Ibrahim Hamitouche</v>
+      </c>
+      <c r="B48" s="6">
         <v>1</v>
       </c>
-      <c r="D48" s="6"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f t="shared" si="5"/>
-        <v>nom4</v>
-      </c>
-      <c r="B49" s="8">
+        <f>B59</f>
+        <v>toto</v>
+      </c>
+      <c r="B49" s="6">
         <v>1</v>
       </c>
-      <c r="D49" s="6"/>
-    </row>
-    <row r="50" spans="1:4" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="B50" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B50" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+    </row>
+    <row r="51" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>B56</f>
-        <v>nom1</v>
-      </c>
-      <c r="B52" s="8">
-        <v>1</v>
-      </c>
-      <c r="D52" s="6"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Patrick Messier</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f t="shared" ref="A53:A55" si="6">B57</f>
-        <v>nom2</v>
-      </c>
-      <c r="B53" s="8">
-        <v>1</v>
-      </c>
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" ref="A53" si="1">B57</f>
+        <v>Rose Duval</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f t="shared" si="6"/>
-        <v>nom3</v>
-      </c>
-      <c r="B54" s="8">
-        <v>1</v>
-      </c>
-      <c r="D54" s="6"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <f>B58</f>
+        <v>Ibrahim Hamitouche</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f t="shared" si="6"/>
-        <v>nom4</v>
-      </c>
-      <c r="B55" s="8">
-        <v>1</v>
-      </c>
-      <c r="D55" s="6"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <f>B59</f>
+        <v>toto</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B56" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B57" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="7" t="s">
-        <v>8</v>
+      <c r="B59" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B38:D38"/>
     <mergeCell ref="B50:D50"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>